<commit_message>
Sun Dec 26 13:11:39 CST 2021
</commit_message>
<xml_diff>
--- a/笔记/CBAP/知识点.xlsx
+++ b/笔记/CBAP/知识点.xlsx
@@ -1901,12 +1901,20 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
       <t>Change</t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t>: the act of transformation in response to a need.</t>
@@ -1914,12 +1922,20 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
       <t>Need</t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t>: a problem or opportunity to be addressed.</t>
@@ -1927,12 +1943,20 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
       <t>Solution</t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t>: a specific way of satisfying one or more needs in a context.</t>
@@ -1940,12 +1964,20 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
       <t>Stakeholder</t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t>: a group or individual with a relationship to the change, the need, or the solution.</t>
@@ -1953,12 +1985,20 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
       <t>Value</t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t>: the worth, importance, or usefulness of something to a stakeholder within a context.</t>
@@ -1966,12 +2006,20 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
       <t>Context</t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t>: the circumstances that influence, are influenced by, and provide understanding of the 
@@ -8658,10 +8706,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="33">
     <font>
@@ -8715,13 +8763,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -8736,9 +8777,69 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -8752,32 +8853,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -8798,61 +8898,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -8926,12 +8974,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -8944,19 +8986,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -8968,25 +9016,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -9004,13 +9058,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -9022,43 +9124,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -9070,43 +9136,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -9309,8 +9357,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -9326,6 +9374,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -9359,166 +9416,157 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="28" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="18" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="18" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="24" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -9717,20 +9765,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -9745,9 +9781,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -10213,420 +10246,424 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A28" sqref="A28"/>
+      <selection pane="bottomLeft" activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.703125" defaultRowHeight="40" customHeight="1" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="24.375" style="71" customWidth="1"/>
-    <col min="2" max="3" width="20.703125" style="71" customWidth="1"/>
-    <col min="4" max="4" width="21.75" style="71" customWidth="1"/>
-    <col min="5" max="16384" width="20.703125" style="71" customWidth="1"/>
+    <col min="1" max="1" width="24.375" style="67" customWidth="1"/>
+    <col min="2" max="3" width="20.703125" style="67" customWidth="1"/>
+    <col min="4" max="4" width="21.75" style="67" customWidth="1"/>
+    <col min="5" max="16384" width="20.703125" style="67" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" customHeight="1" spans="1:4">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="72" t="s">
+      <c r="B1" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="72" t="s">
+      <c r="C1" s="68" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="72" t="s">
+      <c r="D1" s="68" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customHeight="1" spans="1:4">
-      <c r="A2" s="73" t="s">
+      <c r="A2" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="74"/>
-      <c r="C2" s="74"/>
-      <c r="D2" s="75"/>
+      <c r="B2" s="70"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="71"/>
     </row>
     <row r="3" customHeight="1" spans="1:4">
-      <c r="A3" s="76" t="s">
+      <c r="A3" s="72" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="75"/>
-      <c r="C3" s="75"/>
-      <c r="D3" s="75"/>
+      <c r="B3" s="71"/>
+      <c r="C3" s="71"/>
+      <c r="D3" s="71"/>
     </row>
     <row r="4" customHeight="1" spans="1:4">
-      <c r="A4" s="76" t="s">
+      <c r="A4" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="75"/>
-      <c r="C4" s="75"/>
-      <c r="D4" s="75"/>
+      <c r="B4" s="71"/>
+      <c r="C4" s="71"/>
+      <c r="D4" s="71"/>
     </row>
     <row r="5" customHeight="1" spans="1:4">
-      <c r="A5" s="76" t="s">
+      <c r="A5" s="72" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="75"/>
-      <c r="C5" s="75"/>
-      <c r="D5" s="75"/>
+      <c r="B5" s="71"/>
+      <c r="C5" s="71"/>
+      <c r="D5" s="71"/>
     </row>
     <row r="6" customHeight="1" spans="1:4">
-      <c r="A6" s="76" t="s">
+      <c r="A6" s="72" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="75"/>
-      <c r="C6" s="75"/>
-      <c r="D6" s="75"/>
+      <c r="B6" s="71"/>
+      <c r="C6" s="71"/>
+      <c r="D6" s="71"/>
     </row>
     <row r="7" customHeight="1" spans="1:4">
-      <c r="A7" s="76" t="s">
+      <c r="A7" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="75"/>
-      <c r="C7" s="75"/>
-      <c r="D7" s="75"/>
+      <c r="B7" s="71"/>
+      <c r="C7" s="71"/>
+      <c r="D7" s="71"/>
     </row>
     <row r="8" customHeight="1" spans="1:4">
-      <c r="A8" s="76" t="s">
+      <c r="A8" s="72" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="75"/>
-      <c r="C8" s="75"/>
-      <c r="D8" s="75"/>
+      <c r="B8" s="71"/>
+      <c r="C8" s="71"/>
+      <c r="D8" s="71"/>
     </row>
     <row r="9" customHeight="1" spans="1:4">
-      <c r="A9" s="76" t="s">
+      <c r="A9" s="72" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="75"/>
-      <c r="C9" s="75">
+      <c r="B9" s="71"/>
+      <c r="C9" s="71">
         <v>20211106</v>
       </c>
-      <c r="D9" s="75"/>
+      <c r="D9" s="71"/>
     </row>
     <row r="10" customHeight="1" spans="1:4">
-      <c r="A10" s="76" t="s">
+      <c r="A10" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="75"/>
-      <c r="C10" s="75">
+      <c r="B10" s="71"/>
+      <c r="C10" s="71">
         <v>20211114</v>
       </c>
-      <c r="D10" s="75"/>
+      <c r="D10" s="71"/>
     </row>
     <row r="11" customHeight="1" spans="1:4">
-      <c r="A11" s="76" t="s">
+      <c r="A11" s="72" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="75"/>
-      <c r="C11" s="75">
+      <c r="B11" s="71"/>
+      <c r="C11" s="71">
         <v>20211208</v>
       </c>
-      <c r="D11" s="75"/>
+      <c r="D11" s="71"/>
     </row>
     <row r="12" customHeight="1" spans="1:4">
-      <c r="A12" s="76" t="s">
+      <c r="A12" s="72" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="75"/>
-      <c r="C12" s="75">
+      <c r="B12" s="71"/>
+      <c r="C12" s="71">
         <v>20211225</v>
       </c>
-      <c r="D12" s="75"/>
+      <c r="D12" s="71"/>
     </row>
     <row r="13" customHeight="1" spans="1:4">
-      <c r="A13" s="76" t="s">
+      <c r="A13" s="72" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="75"/>
-      <c r="C13" s="75">
+      <c r="B13" s="71"/>
+      <c r="C13" s="71">
         <v>20211106</v>
       </c>
-      <c r="D13" s="75"/>
+      <c r="D13" s="71"/>
     </row>
     <row r="14" customHeight="1" spans="1:4">
-      <c r="A14" s="76" t="s">
+      <c r="A14" s="72" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="75"/>
-      <c r="C14" s="75">
+      <c r="B14" s="71"/>
+      <c r="C14" s="71">
         <v>20211106</v>
       </c>
-      <c r="D14" s="75"/>
+      <c r="D14" s="71"/>
     </row>
     <row r="15" customHeight="1" spans="1:4">
-      <c r="A15" s="76" t="s">
+      <c r="A15" s="72" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="75"/>
-      <c r="C15" s="75">
+      <c r="B15" s="71"/>
+      <c r="C15" s="71">
         <v>20211108</v>
       </c>
-      <c r="D15" s="75"/>
+      <c r="D15" s="71"/>
     </row>
     <row r="16" customHeight="1" spans="1:4">
-      <c r="A16" s="76" t="s">
+      <c r="A16" s="72" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="75"/>
-      <c r="C16" s="75">
+      <c r="B16" s="71"/>
+      <c r="C16" s="71">
         <v>20211108</v>
       </c>
-      <c r="D16" s="75"/>
+      <c r="D16" s="71"/>
     </row>
     <row r="17" customHeight="1" spans="1:4">
-      <c r="A17" s="76" t="s">
+      <c r="A17" s="72" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="75"/>
-      <c r="C17" s="75">
+      <c r="B17" s="71"/>
+      <c r="C17" s="71">
         <v>20211108</v>
       </c>
-      <c r="D17" s="75"/>
+      <c r="D17" s="71"/>
     </row>
     <row r="18" customHeight="1" spans="1:4">
-      <c r="A18" s="76" t="s">
+      <c r="A18" s="72" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="75"/>
-      <c r="C18" s="75">
+      <c r="B18" s="71"/>
+      <c r="C18" s="71">
         <v>20211109</v>
       </c>
-      <c r="D18" s="75"/>
+      <c r="D18" s="71"/>
     </row>
     <row r="19" customHeight="1" spans="1:4">
-      <c r="A19" s="76" t="s">
+      <c r="A19" s="72" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="75"/>
-      <c r="C19" s="75">
+      <c r="B19" s="71"/>
+      <c r="C19" s="71">
         <v>20211109</v>
       </c>
-      <c r="D19" s="75"/>
+      <c r="D19" s="71"/>
     </row>
     <row r="20" customHeight="1" spans="1:4">
-      <c r="A20" s="76" t="s">
+      <c r="A20" s="72" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="75"/>
-      <c r="C20" s="75">
+      <c r="B20" s="71"/>
+      <c r="C20" s="71">
         <v>20211109</v>
       </c>
-      <c r="D20" s="75"/>
+      <c r="D20" s="71"/>
     </row>
     <row r="21" customHeight="1" spans="1:4">
-      <c r="A21" s="76" t="s">
+      <c r="A21" s="72" t="s">
         <v>23</v>
       </c>
-      <c r="B21" s="75"/>
-      <c r="C21" s="75">
+      <c r="B21" s="71"/>
+      <c r="C21" s="71">
         <v>20211114</v>
       </c>
-      <c r="D21" s="75"/>
+      <c r="D21" s="71"/>
     </row>
     <row r="22" customHeight="1" spans="1:4">
-      <c r="A22" s="76" t="s">
+      <c r="A22" s="72" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="75"/>
-      <c r="C22" s="75">
+      <c r="B22" s="71"/>
+      <c r="C22" s="71">
         <v>20211208</v>
       </c>
-      <c r="D22" s="75"/>
+      <c r="D22" s="71"/>
     </row>
     <row r="23" customHeight="1" spans="1:4">
-      <c r="A23" s="76" t="s">
+      <c r="A23" s="72" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="75"/>
-      <c r="C23" s="75">
+      <c r="B23" s="71"/>
+      <c r="C23" s="71">
         <v>20211225</v>
       </c>
-      <c r="D23" s="75"/>
+      <c r="D23" s="71"/>
     </row>
     <row r="24" customHeight="1" spans="1:4">
-      <c r="A24" s="76" t="s">
+      <c r="A24" s="72" t="s">
         <v>26</v>
       </c>
-      <c r="B24" s="76"/>
-      <c r="C24" s="76"/>
-      <c r="D24" s="76" t="s">
+      <c r="B24" s="72"/>
+      <c r="C24" s="72"/>
+      <c r="D24" s="72" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="25" customHeight="1" spans="1:4">
-      <c r="A25" s="76" t="s">
+      <c r="A25" s="72" t="s">
         <v>28</v>
       </c>
-      <c r="B25" s="76"/>
-      <c r="C25" s="76"/>
-      <c r="D25" s="76" t="s">
+      <c r="B25" s="72"/>
+      <c r="C25" s="72"/>
+      <c r="D25" s="72" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="26" customHeight="1" spans="1:4">
-      <c r="A26" s="76" t="s">
+      <c r="A26" s="72" t="s">
         <v>30</v>
       </c>
-      <c r="B26" s="75"/>
-      <c r="C26" s="75">
+      <c r="B26" s="71"/>
+      <c r="C26" s="71">
         <v>20211225</v>
       </c>
-      <c r="D26" s="75" t="s">
+      <c r="D26" s="71" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="27" customHeight="1" spans="1:4">
-      <c r="A27" s="76" t="s">
+      <c r="A27" s="72" t="s">
         <v>32</v>
       </c>
-      <c r="B27" s="76"/>
-      <c r="C27" s="76"/>
-      <c r="D27" s="76"/>
+      <c r="B27" s="71"/>
+      <c r="C27" s="71">
+        <v>20211226</v>
+      </c>
+      <c r="D27" s="71"/>
     </row>
     <row r="28" customHeight="1" spans="1:4">
-      <c r="A28" s="76" t="s">
+      <c r="A28" s="72" t="s">
         <v>33</v>
       </c>
-      <c r="B28" s="76"/>
-      <c r="C28" s="76"/>
-      <c r="D28" s="76"/>
+      <c r="B28" s="71"/>
+      <c r="C28" s="71">
+        <v>20211226</v>
+      </c>
+      <c r="D28" s="71"/>
     </row>
     <row r="29" customHeight="1" spans="1:4">
-      <c r="A29" s="76" t="s">
+      <c r="A29" s="72" t="s">
         <v>34</v>
       </c>
-      <c r="B29" s="76"/>
-      <c r="C29" s="76"/>
-      <c r="D29" s="76"/>
+      <c r="B29" s="72"/>
+      <c r="C29" s="72"/>
+      <c r="D29" s="72"/>
     </row>
     <row r="30" customHeight="1" spans="1:4">
-      <c r="A30" s="76" t="s">
+      <c r="A30" s="72" t="s">
         <v>35</v>
       </c>
-      <c r="B30" s="76"/>
-      <c r="C30" s="76"/>
-      <c r="D30" s="76"/>
+      <c r="B30" s="72"/>
+      <c r="C30" s="72"/>
+      <c r="D30" s="72"/>
     </row>
     <row r="31" customHeight="1" spans="1:4">
-      <c r="A31" s="76" t="s">
+      <c r="A31" s="72" t="s">
         <v>36</v>
       </c>
-      <c r="B31" s="76"/>
-      <c r="C31" s="76"/>
-      <c r="D31" s="76"/>
+      <c r="B31" s="72"/>
+      <c r="C31" s="72"/>
+      <c r="D31" s="72"/>
     </row>
     <row r="32" customHeight="1" spans="1:4">
-      <c r="A32" s="76" t="s">
+      <c r="A32" s="72" t="s">
         <v>37</v>
       </c>
-      <c r="B32" s="76"/>
-      <c r="C32" s="76"/>
-      <c r="D32" s="76"/>
+      <c r="B32" s="72"/>
+      <c r="C32" s="72"/>
+      <c r="D32" s="72"/>
     </row>
     <row r="33" customHeight="1" spans="1:4">
-      <c r="A33" s="76" t="s">
+      <c r="A33" s="72" t="s">
         <v>38</v>
       </c>
-      <c r="B33" s="76"/>
-      <c r="C33" s="76"/>
-      <c r="D33" s="76"/>
+      <c r="B33" s="72"/>
+      <c r="C33" s="72"/>
+      <c r="D33" s="72"/>
     </row>
     <row r="34" customHeight="1" spans="1:4">
-      <c r="A34" s="76" t="s">
+      <c r="A34" s="72" t="s">
         <v>39</v>
       </c>
-      <c r="B34" s="76"/>
-      <c r="C34" s="76"/>
-      <c r="D34" s="76"/>
+      <c r="B34" s="72"/>
+      <c r="C34" s="72"/>
+      <c r="D34" s="72"/>
     </row>
     <row r="35" customHeight="1" spans="1:4">
-      <c r="A35" s="76" t="s">
+      <c r="A35" s="72" t="s">
         <v>40</v>
       </c>
-      <c r="B35" s="77"/>
-      <c r="C35" s="77"/>
-      <c r="D35" s="77"/>
+      <c r="B35" s="72"/>
+      <c r="C35" s="72"/>
+      <c r="D35" s="72"/>
     </row>
     <row r="36" customHeight="1" spans="1:4">
-      <c r="A36" s="76" t="s">
+      <c r="A36" s="72" t="s">
         <v>41</v>
       </c>
-      <c r="B36" s="77"/>
-      <c r="C36" s="77"/>
-      <c r="D36" s="77"/>
+      <c r="B36" s="72"/>
+      <c r="C36" s="72"/>
+      <c r="D36" s="72"/>
     </row>
     <row r="37" customHeight="1" spans="1:4">
-      <c r="A37" s="76" t="s">
+      <c r="A37" s="72" t="s">
         <v>42</v>
       </c>
-      <c r="B37" s="77"/>
-      <c r="C37" s="77"/>
-      <c r="D37" s="77"/>
+      <c r="B37" s="72"/>
+      <c r="C37" s="72"/>
+      <c r="D37" s="72"/>
     </row>
     <row r="38" customHeight="1" spans="1:4">
-      <c r="A38" s="76" t="s">
+      <c r="A38" s="72" t="s">
         <v>43</v>
       </c>
-      <c r="B38" s="77"/>
-      <c r="C38" s="77"/>
-      <c r="D38" s="77"/>
+      <c r="B38" s="72"/>
+      <c r="C38" s="72"/>
+      <c r="D38" s="72"/>
     </row>
     <row r="39" customHeight="1" spans="1:4">
-      <c r="A39" s="76" t="s">
+      <c r="A39" s="72" t="s">
         <v>44</v>
       </c>
-      <c r="B39" s="77"/>
-      <c r="C39" s="77"/>
-      <c r="D39" s="77"/>
+      <c r="B39" s="72"/>
+      <c r="C39" s="72"/>
+      <c r="D39" s="72"/>
     </row>
     <row r="40" customHeight="1" spans="1:4">
-      <c r="A40" s="76" t="s">
+      <c r="A40" s="72" t="s">
         <v>45</v>
       </c>
-      <c r="B40" s="77"/>
-      <c r="C40" s="77"/>
-      <c r="D40" s="77"/>
+      <c r="B40" s="72"/>
+      <c r="C40" s="72"/>
+      <c r="D40" s="72"/>
     </row>
     <row r="41" customHeight="1" spans="1:4">
-      <c r="A41" s="76" t="s">
+      <c r="A41" s="72" t="s">
         <v>46</v>
       </c>
-      <c r="B41" s="77"/>
-      <c r="C41" s="77"/>
-      <c r="D41" s="77"/>
+      <c r="B41" s="72"/>
+      <c r="C41" s="72"/>
+      <c r="D41" s="72"/>
     </row>
     <row r="42" customHeight="1" spans="1:4">
-      <c r="A42" s="76" t="s">
+      <c r="A42" s="72" t="s">
         <v>47</v>
       </c>
-      <c r="B42" s="77"/>
-      <c r="C42" s="77"/>
-      <c r="D42" s="77"/>
+      <c r="B42" s="72"/>
+      <c r="C42" s="72"/>
+      <c r="D42" s="72"/>
     </row>
     <row r="43" customHeight="1" spans="1:4">
-      <c r="A43" s="76" t="s">
+      <c r="A43" s="72" t="s">
         <v>48</v>
       </c>
-      <c r="B43" s="77"/>
-      <c r="C43" s="77"/>
-      <c r="D43" s="77"/>
+      <c r="B43" s="72"/>
+      <c r="C43" s="72"/>
+      <c r="D43" s="72"/>
     </row>
     <row r="44" customHeight="1" spans="1:4">
-      <c r="A44" s="76" t="s">
+      <c r="A44" s="72" t="s">
         <v>49</v>
       </c>
-      <c r="B44" s="77"/>
-      <c r="C44" s="77"/>
-      <c r="D44" s="77"/>
+      <c r="B44" s="72"/>
+      <c r="C44" s="72"/>
+      <c r="D44" s="72"/>
     </row>
     <row r="45" customHeight="1" spans="1:4">
-      <c r="A45" s="76" t="s">
+      <c r="A45" s="72" t="s">
         <v>50</v>
       </c>
-      <c r="B45" s="77"/>
-      <c r="C45" s="77"/>
-      <c r="D45" s="77"/>
+      <c r="B45" s="72"/>
+      <c r="C45" s="72"/>
+      <c r="D45" s="72"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
@@ -17414,54 +17451,54 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelRow="6" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="37.890625" style="66" customWidth="1"/>
-    <col min="2" max="2" width="36.328125" style="66" customWidth="1"/>
-    <col min="3" max="16384" width="9" style="67"/>
+    <col min="1" max="1" width="37.890625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="36.328125" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="1" customHeight="1" spans="1:2">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="66" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="68" t="s">
+      <c r="B1" s="66" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="2" customHeight="1" spans="1:2">
-      <c r="A2" s="69" t="s">
+      <c r="A2" s="54" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="70"/>
+      <c r="B2" s="7"/>
     </row>
     <row r="3" customHeight="1" spans="1:2">
-      <c r="A3" s="69" t="s">
+      <c r="A3" s="54" t="s">
         <v>54</v>
       </c>
-      <c r="B3" s="70"/>
+      <c r="B3" s="7"/>
     </row>
     <row r="4" ht="54" customHeight="1" spans="1:2">
-      <c r="A4" s="69" t="s">
+      <c r="A4" s="54" t="s">
         <v>55</v>
       </c>
-      <c r="B4" s="70"/>
+      <c r="B4" s="7"/>
     </row>
     <row r="5" ht="54" customHeight="1" spans="1:2">
-      <c r="A5" s="69" t="s">
+      <c r="A5" s="54" t="s">
         <v>56</v>
       </c>
-      <c r="B5" s="70"/>
+      <c r="B5" s="7"/>
     </row>
     <row r="6" ht="49" customHeight="1" spans="1:2">
-      <c r="A6" s="69" t="s">
+      <c r="A6" s="54" t="s">
         <v>57</v>
       </c>
-      <c r="B6" s="70"/>
+      <c r="B6" s="7"/>
     </row>
     <row r="7" ht="49" customHeight="1" spans="1:2">
-      <c r="A7" s="69" t="s">
+      <c r="A7" s="54" t="s">
         <v>58</v>
       </c>
-      <c r="B7" s="70"/>
+      <c r="B7" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
@@ -17475,7 +17512,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.0859375" defaultRowHeight="40" customHeight="1" outlineLevelCol="3"/>

</xml_diff>

<commit_message>
Thu Dec 30 02:04:26 CST 2021
</commit_message>
<xml_diff>
--- a/笔记/CBAP/知识点.xlsx
+++ b/笔记/CBAP/知识点.xlsx
@@ -8707,9 +8707,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="33">
     <font>
@@ -8771,7 +8771,23 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -8785,7 +8801,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -8800,6 +8816,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -8807,24 +8831,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -8839,7 +8847,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -8853,16 +8876,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -8875,24 +8891,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -8900,7 +8900,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -8980,25 +8980,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -9016,13 +9022,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -9034,19 +9130,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -9058,103 +9148,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -9319,16 +9319,16 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="double">
+      <right style="thin">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="double">
+      <top style="thin">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
+      <bottom style="thin">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -9338,17 +9338,6 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -9380,9 +9369,35 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -9401,159 +9416,144 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="17" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="31" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="6" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="28" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="18" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="28" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -9562,11 +9562,11 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -9784,6 +9784,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -10244,9 +10247,9 @@
   <dimension ref="A1:D45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D28" sqref="D28"/>
+      <selection pane="bottomLeft" activeCell="B37" sqref="B37:C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.703125" defaultRowHeight="40" customHeight="1" outlineLevelCol="3"/>
@@ -10581,24 +10584,28 @@
       <c r="A35" s="72" t="s">
         <v>40</v>
       </c>
-      <c r="B35" s="72"/>
-      <c r="C35" s="72"/>
+      <c r="B35" s="71"/>
+      <c r="C35" s="71">
+        <v>20211229</v>
+      </c>
       <c r="D35" s="72"/>
     </row>
     <row r="36" customHeight="1" spans="1:4">
       <c r="A36" s="72" t="s">
         <v>41</v>
       </c>
-      <c r="B36" s="72"/>
-      <c r="C36" s="72"/>
+      <c r="B36" s="71"/>
+      <c r="C36" s="71">
+        <v>20211229</v>
+      </c>
       <c r="D36" s="72"/>
     </row>
     <row r="37" customHeight="1" spans="1:4">
       <c r="A37" s="72" t="s">
         <v>42</v>
       </c>
-      <c r="B37" s="72"/>
-      <c r="C37" s="72"/>
+      <c r="B37" s="73"/>
+      <c r="C37" s="73"/>
       <c r="D37" s="72"/>
     </row>
     <row r="38" customHeight="1" spans="1:4">

</xml_diff>

<commit_message>
Mon Jan  3 00:28:03 CST 2022
</commit_message>
<xml_diff>
--- a/笔记/CBAP/知识点.xlsx
+++ b/笔记/CBAP/知识点.xlsx
@@ -8762,8 +8762,70 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -8777,17 +8839,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -8800,15 +8853,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="18"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -8817,17 +8863,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -8838,16 +8876,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -8860,39 +8890,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -8900,7 +8900,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -8974,19 +8974,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -8998,7 +8992,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -9016,19 +9010,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -9040,19 +9034,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -9070,7 +9052,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -9082,73 +9136,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -9319,17 +9319,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
+      <right style="double">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
+      <top style="double">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
+      <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -9343,11 +9352,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -9367,13 +9382,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -9387,32 +9406,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
       </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -9421,152 +9421,152 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="17" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="18" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="31" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="6" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -9784,9 +9784,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -10247,9 +10244,9 @@
   <dimension ref="A1:D45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B37" sqref="B37:C37"/>
+      <selection pane="bottomLeft" activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.703125" defaultRowHeight="40" customHeight="1" outlineLevelCol="3"/>
@@ -10604,16 +10601,20 @@
       <c r="A37" s="72" t="s">
         <v>42</v>
       </c>
-      <c r="B37" s="73"/>
-      <c r="C37" s="73"/>
+      <c r="B37" s="71"/>
+      <c r="C37" s="71">
+        <v>20211230</v>
+      </c>
       <c r="D37" s="72"/>
     </row>
     <row r="38" customHeight="1" spans="1:4">
       <c r="A38" s="72" t="s">
         <v>43</v>
       </c>
-      <c r="B38" s="72"/>
-      <c r="C38" s="72"/>
+      <c r="B38" s="71"/>
+      <c r="C38" s="71">
+        <v>20220101</v>
+      </c>
       <c r="D38" s="72"/>
     </row>
     <row r="39" customHeight="1" spans="1:4">

</xml_diff>

<commit_message>
Mon Jan  3 03:18:51 CST 2022
</commit_message>
<xml_diff>
--- a/笔记/CBAP/知识点.xlsx
+++ b/笔记/CBAP/知识点.xlsx
@@ -10244,9 +10244,9 @@
   <dimension ref="A1:D45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D38" sqref="D38"/>
+      <selection pane="bottomLeft" activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.703125" defaultRowHeight="40" customHeight="1" outlineLevelCol="3"/>
@@ -10621,8 +10621,10 @@
       <c r="A39" s="72" t="s">
         <v>44</v>
       </c>
-      <c r="B39" s="72"/>
-      <c r="C39" s="72"/>
+      <c r="B39" s="71"/>
+      <c r="C39" s="71">
+        <v>20220102</v>
+      </c>
       <c r="D39" s="72"/>
     </row>
     <row r="40" customHeight="1" spans="1:4">

</xml_diff>

<commit_message>
Mon Jan 10 02:55:53 CST 2022
</commit_message>
<xml_diff>
--- a/笔记/CBAP/知识点.xlsx
+++ b/笔记/CBAP/知识点.xlsx
@@ -10244,9 +10244,9 @@
   <dimension ref="A1:D45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C41" sqref="C41"/>
+      <selection pane="bottomLeft" activeCell="B41" sqref="B41:C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.703125" defaultRowHeight="40" customHeight="1" outlineLevelCol="3"/>
@@ -10641,16 +10641,20 @@
       <c r="A41" s="72" t="s">
         <v>46</v>
       </c>
-      <c r="B41" s="72"/>
-      <c r="C41" s="72"/>
+      <c r="B41" s="71"/>
+      <c r="C41" s="71">
+        <v>20220108</v>
+      </c>
       <c r="D41" s="72"/>
     </row>
     <row r="42" customHeight="1" spans="1:4">
       <c r="A42" s="72" t="s">
         <v>47</v>
       </c>
-      <c r="B42" s="72"/>
-      <c r="C42" s="72"/>
+      <c r="B42" s="71"/>
+      <c r="C42" s="71">
+        <v>20220108</v>
+      </c>
       <c r="D42" s="72"/>
     </row>
     <row r="43" customHeight="1" spans="1:4">

</xml_diff>

<commit_message>
Sun Mar 27 09:23:40 CST 2022
</commit_message>
<xml_diff>
--- a/笔记/CBAP/知识点.xlsx
+++ b/笔记/CBAP/知识点.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="13180" activeTab="4"/>
+    <workbookView windowWidth="28800" windowHeight="13180" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="核查单" sheetId="12" r:id="rId1"/>
@@ -10141,9 +10141,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="33">
@@ -10205,8 +10205,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -10221,34 +10222,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -10267,11 +10244,47 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -10290,8 +10303,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -10305,30 +10327,8 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -10409,13 +10409,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -10427,103 +10565,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -10535,61 +10583,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -10773,7 +10773,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -10797,7 +10797,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -10819,20 +10819,20 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -10856,142 +10856,142 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="21" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="21" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="13" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -11001,7 +11001,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -11206,9 +11206,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -11306,6 +11303,53 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>854710</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>785495</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>149860</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1" r:link="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="26100405" y="3949700"/>
+          <a:ext cx="4470400" cy="4467860"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -11704,471 +11748,471 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.703125" defaultRowHeight="40" customHeight="1" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="24.375" style="72" customWidth="1"/>
-    <col min="2" max="3" width="20.703125" style="72" customWidth="1"/>
-    <col min="4" max="4" width="21.75" style="72" customWidth="1"/>
-    <col min="5" max="16384" width="20.703125" style="72" customWidth="1"/>
+    <col min="1" max="1" width="24.375" style="71" customWidth="1"/>
+    <col min="2" max="3" width="20.703125" style="71" customWidth="1"/>
+    <col min="4" max="4" width="21.75" style="71" customWidth="1"/>
+    <col min="5" max="16384" width="20.703125" style="71" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" customHeight="1" spans="1:4">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="73" t="s">
+      <c r="B1" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="73" t="s">
+      <c r="C1" s="72" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="73" t="s">
+      <c r="D1" s="72" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customHeight="1" spans="1:4">
-      <c r="A2" s="74" t="s">
+      <c r="A2" s="73" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="75"/>
-      <c r="C2" s="75"/>
-      <c r="D2" s="76"/>
+      <c r="B2" s="74"/>
+      <c r="C2" s="74"/>
+      <c r="D2" s="75"/>
     </row>
     <row r="3" customHeight="1" spans="1:4">
-      <c r="A3" s="77" t="s">
+      <c r="A3" s="76" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="76"/>
-      <c r="C3" s="76"/>
-      <c r="D3" s="76"/>
+      <c r="B3" s="75"/>
+      <c r="C3" s="75"/>
+      <c r="D3" s="75"/>
     </row>
     <row r="4" customHeight="1" spans="1:4">
-      <c r="A4" s="77" t="s">
+      <c r="A4" s="76" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="76"/>
-      <c r="C4" s="76"/>
-      <c r="D4" s="76"/>
+      <c r="B4" s="75"/>
+      <c r="C4" s="75"/>
+      <c r="D4" s="75"/>
     </row>
     <row r="5" customHeight="1" spans="1:4">
-      <c r="A5" s="77" t="s">
+      <c r="A5" s="76" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="76"/>
-      <c r="C5" s="76"/>
-      <c r="D5" s="76"/>
+      <c r="B5" s="75"/>
+      <c r="C5" s="75"/>
+      <c r="D5" s="75"/>
     </row>
     <row r="6" customHeight="1" spans="1:4">
-      <c r="A6" s="77" t="s">
+      <c r="A6" s="76" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="76"/>
-      <c r="C6" s="76"/>
-      <c r="D6" s="76"/>
+      <c r="B6" s="75"/>
+      <c r="C6" s="75"/>
+      <c r="D6" s="75"/>
     </row>
     <row r="7" customHeight="1" spans="1:4">
-      <c r="A7" s="77" t="s">
+      <c r="A7" s="76" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="76"/>
-      <c r="C7" s="76"/>
-      <c r="D7" s="76"/>
+      <c r="B7" s="75"/>
+      <c r="C7" s="75"/>
+      <c r="D7" s="75"/>
     </row>
     <row r="8" customHeight="1" spans="1:4">
-      <c r="A8" s="77" t="s">
+      <c r="A8" s="76" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="76"/>
-      <c r="C8" s="76"/>
-      <c r="D8" s="76"/>
+      <c r="B8" s="75"/>
+      <c r="C8" s="75"/>
+      <c r="D8" s="75"/>
     </row>
     <row r="9" customHeight="1" spans="1:4">
-      <c r="A9" s="77" t="s">
+      <c r="A9" s="76" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="76"/>
-      <c r="C9" s="76">
+      <c r="B9" s="75"/>
+      <c r="C9" s="75">
         <v>20211106</v>
       </c>
-      <c r="D9" s="76"/>
+      <c r="D9" s="75"/>
     </row>
     <row r="10" customHeight="1" spans="1:4">
-      <c r="A10" s="77" t="s">
+      <c r="A10" s="76" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="76"/>
-      <c r="C10" s="76">
+      <c r="B10" s="75"/>
+      <c r="C10" s="75">
         <v>20211114</v>
       </c>
-      <c r="D10" s="76"/>
+      <c r="D10" s="75"/>
     </row>
     <row r="11" customHeight="1" spans="1:4">
-      <c r="A11" s="77" t="s">
+      <c r="A11" s="76" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="76"/>
-      <c r="C11" s="76">
+      <c r="B11" s="75"/>
+      <c r="C11" s="75">
         <v>20211208</v>
       </c>
-      <c r="D11" s="76"/>
+      <c r="D11" s="75"/>
     </row>
     <row r="12" customHeight="1" spans="1:4">
-      <c r="A12" s="77" t="s">
+      <c r="A12" s="76" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="76"/>
-      <c r="C12" s="76">
+      <c r="B12" s="75"/>
+      <c r="C12" s="75">
         <v>20211225</v>
       </c>
-      <c r="D12" s="76"/>
+      <c r="D12" s="75"/>
     </row>
     <row r="13" customHeight="1" spans="1:4">
-      <c r="A13" s="77" t="s">
+      <c r="A13" s="76" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="76"/>
-      <c r="C13" s="76">
+      <c r="B13" s="75"/>
+      <c r="C13" s="75">
         <v>20211106</v>
       </c>
-      <c r="D13" s="76"/>
+      <c r="D13" s="75"/>
     </row>
     <row r="14" customHeight="1" spans="1:4">
-      <c r="A14" s="77" t="s">
+      <c r="A14" s="76" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="76"/>
-      <c r="C14" s="76">
+      <c r="B14" s="75"/>
+      <c r="C14" s="75">
         <v>20211106</v>
       </c>
-      <c r="D14" s="76"/>
+      <c r="D14" s="75"/>
     </row>
     <row r="15" customHeight="1" spans="1:4">
-      <c r="A15" s="77" t="s">
+      <c r="A15" s="76" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="76"/>
-      <c r="C15" s="76">
+      <c r="B15" s="75"/>
+      <c r="C15" s="75">
         <v>20211108</v>
       </c>
-      <c r="D15" s="76"/>
+      <c r="D15" s="75"/>
     </row>
     <row r="16" customHeight="1" spans="1:4">
-      <c r="A16" s="77" t="s">
+      <c r="A16" s="76" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="76"/>
-      <c r="C16" s="76">
+      <c r="B16" s="75"/>
+      <c r="C16" s="75">
         <v>20211108</v>
       </c>
-      <c r="D16" s="76"/>
+      <c r="D16" s="75"/>
     </row>
     <row r="17" customHeight="1" spans="1:4">
-      <c r="A17" s="77" t="s">
+      <c r="A17" s="76" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="76"/>
-      <c r="C17" s="76">
+      <c r="B17" s="75"/>
+      <c r="C17" s="75">
         <v>20211108</v>
       </c>
-      <c r="D17" s="76"/>
+      <c r="D17" s="75"/>
     </row>
     <row r="18" customHeight="1" spans="1:4">
-      <c r="A18" s="77" t="s">
+      <c r="A18" s="76" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="76"/>
-      <c r="C18" s="76">
+      <c r="B18" s="75"/>
+      <c r="C18" s="75">
         <v>20211109</v>
       </c>
-      <c r="D18" s="76"/>
+      <c r="D18" s="75"/>
     </row>
     <row r="19" customHeight="1" spans="1:4">
-      <c r="A19" s="77" t="s">
+      <c r="A19" s="76" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="76"/>
-      <c r="C19" s="76">
+      <c r="B19" s="75"/>
+      <c r="C19" s="75">
         <v>20211109</v>
       </c>
-      <c r="D19" s="76"/>
+      <c r="D19" s="75"/>
     </row>
     <row r="20" customHeight="1" spans="1:4">
-      <c r="A20" s="77" t="s">
+      <c r="A20" s="76" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="76"/>
-      <c r="C20" s="76">
+      <c r="B20" s="75"/>
+      <c r="C20" s="75">
         <v>20211109</v>
       </c>
-      <c r="D20" s="76"/>
+      <c r="D20" s="75"/>
     </row>
     <row r="21" customHeight="1" spans="1:4">
-      <c r="A21" s="77" t="s">
+      <c r="A21" s="76" t="s">
         <v>23</v>
       </c>
-      <c r="B21" s="76"/>
-      <c r="C21" s="76">
+      <c r="B21" s="75"/>
+      <c r="C21" s="75">
         <v>20211114</v>
       </c>
-      <c r="D21" s="76"/>
+      <c r="D21" s="75"/>
     </row>
     <row r="22" customHeight="1" spans="1:4">
-      <c r="A22" s="77" t="s">
+      <c r="A22" s="76" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="76"/>
-      <c r="C22" s="76">
+      <c r="B22" s="75"/>
+      <c r="C22" s="75">
         <v>20211208</v>
       </c>
-      <c r="D22" s="76"/>
+      <c r="D22" s="75"/>
     </row>
     <row r="23" customHeight="1" spans="1:4">
-      <c r="A23" s="77" t="s">
+      <c r="A23" s="76" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="76"/>
-      <c r="C23" s="76">
+      <c r="B23" s="75"/>
+      <c r="C23" s="75">
         <v>20211225</v>
       </c>
-      <c r="D23" s="76"/>
+      <c r="D23" s="75"/>
     </row>
     <row r="24" customHeight="1" spans="1:4">
-      <c r="A24" s="77" t="s">
+      <c r="A24" s="76" t="s">
         <v>26</v>
       </c>
-      <c r="B24" s="76"/>
-      <c r="C24" s="76">
+      <c r="B24" s="75"/>
+      <c r="C24" s="75">
         <v>20220213</v>
       </c>
-      <c r="D24" s="76" t="s">
+      <c r="D24" s="75" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="25" customHeight="1" spans="1:4">
-      <c r="A25" s="77" t="s">
+      <c r="A25" s="76" t="s">
         <v>28</v>
       </c>
-      <c r="B25" s="76"/>
-      <c r="C25" s="76">
+      <c r="B25" s="75"/>
+      <c r="C25" s="75">
         <v>20220213</v>
       </c>
-      <c r="D25" s="76"/>
+      <c r="D25" s="75"/>
     </row>
     <row r="26" customHeight="1" spans="1:4">
-      <c r="A26" s="77" t="s">
+      <c r="A26" s="76" t="s">
         <v>29</v>
       </c>
-      <c r="B26" s="76"/>
-      <c r="C26" s="76">
+      <c r="B26" s="75"/>
+      <c r="C26" s="75">
         <v>20220306</v>
       </c>
-      <c r="D26" s="76"/>
+      <c r="D26" s="75"/>
     </row>
     <row r="27" customHeight="1" spans="1:4">
-      <c r="A27" s="77" t="s">
+      <c r="A27" s="76" t="s">
         <v>30</v>
       </c>
-      <c r="B27" s="78"/>
-      <c r="C27" s="78"/>
-      <c r="D27" s="78"/>
+      <c r="B27" s="77"/>
+      <c r="C27" s="77"/>
+      <c r="D27" s="77"/>
     </row>
     <row r="28" customHeight="1" spans="1:4">
-      <c r="A28" s="77" t="s">
+      <c r="A28" s="76" t="s">
         <v>31</v>
       </c>
-      <c r="B28" s="76"/>
-      <c r="C28" s="76">
+      <c r="B28" s="75"/>
+      <c r="C28" s="75">
         <v>20220320</v>
       </c>
-      <c r="D28" s="76"/>
+      <c r="D28" s="75"/>
     </row>
     <row r="29" customHeight="1" spans="1:4">
-      <c r="A29" s="77" t="s">
+      <c r="A29" s="76" t="s">
         <v>32</v>
       </c>
-      <c r="B29" s="76"/>
-      <c r="C29" s="76">
+      <c r="B29" s="75"/>
+      <c r="C29" s="75">
         <v>20211225</v>
       </c>
-      <c r="D29" s="76" t="s">
+      <c r="D29" s="75" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="30" customHeight="1" spans="1:4">
-      <c r="A30" s="77" t="s">
+      <c r="A30" s="76" t="s">
         <v>34</v>
       </c>
-      <c r="B30" s="76"/>
-      <c r="C30" s="76">
+      <c r="B30" s="75"/>
+      <c r="C30" s="75">
         <v>20211226</v>
       </c>
-      <c r="D30" s="76"/>
+      <c r="D30" s="75"/>
     </row>
     <row r="31" customHeight="1" spans="1:4">
-      <c r="A31" s="77" t="s">
+      <c r="A31" s="76" t="s">
         <v>35</v>
       </c>
-      <c r="B31" s="76"/>
-      <c r="C31" s="76">
+      <c r="B31" s="75"/>
+      <c r="C31" s="75">
         <v>20211226</v>
       </c>
-      <c r="D31" s="76"/>
+      <c r="D31" s="75"/>
     </row>
     <row r="32" customHeight="1" spans="1:4">
-      <c r="A32" s="77" t="s">
+      <c r="A32" s="76" t="s">
         <v>36</v>
       </c>
-      <c r="B32" s="77"/>
-      <c r="C32" s="77"/>
-      <c r="D32" s="77"/>
+      <c r="B32" s="76"/>
+      <c r="C32" s="76"/>
+      <c r="D32" s="76"/>
     </row>
     <row r="33" customHeight="1" spans="1:4">
-      <c r="A33" s="77" t="s">
+      <c r="A33" s="76" t="s">
         <v>37</v>
       </c>
-      <c r="B33" s="77"/>
-      <c r="C33" s="77"/>
-      <c r="D33" s="77"/>
+      <c r="B33" s="76"/>
+      <c r="C33" s="76"/>
+      <c r="D33" s="76"/>
     </row>
     <row r="34" customHeight="1" spans="1:4">
-      <c r="A34" s="77" t="s">
+      <c r="A34" s="76" t="s">
         <v>38</v>
       </c>
-      <c r="B34" s="77"/>
-      <c r="C34" s="77"/>
-      <c r="D34" s="77"/>
+      <c r="B34" s="76"/>
+      <c r="C34" s="76"/>
+      <c r="D34" s="76"/>
     </row>
     <row r="35" customHeight="1" spans="1:4">
-      <c r="A35" s="77" t="s">
+      <c r="A35" s="76" t="s">
         <v>39</v>
       </c>
-      <c r="B35" s="77"/>
-      <c r="C35" s="77"/>
-      <c r="D35" s="77"/>
+      <c r="B35" s="76"/>
+      <c r="C35" s="76"/>
+      <c r="D35" s="76"/>
     </row>
     <row r="36" customHeight="1" spans="1:4">
-      <c r="A36" s="77" t="s">
+      <c r="A36" s="76" t="s">
         <v>40</v>
       </c>
-      <c r="B36" s="77"/>
-      <c r="C36" s="77"/>
-      <c r="D36" s="77"/>
+      <c r="B36" s="76"/>
+      <c r="C36" s="76"/>
+      <c r="D36" s="76"/>
     </row>
     <row r="37" customHeight="1" spans="1:4">
-      <c r="A37" s="77" t="s">
+      <c r="A37" s="76" t="s">
         <v>41</v>
       </c>
-      <c r="B37" s="77"/>
-      <c r="C37" s="77"/>
-      <c r="D37" s="77"/>
+      <c r="B37" s="76"/>
+      <c r="C37" s="76"/>
+      <c r="D37" s="76"/>
     </row>
     <row r="38" customHeight="1" spans="1:4">
-      <c r="A38" s="77" t="s">
+      <c r="A38" s="76" t="s">
         <v>42</v>
       </c>
-      <c r="B38" s="76"/>
-      <c r="C38" s="76">
+      <c r="B38" s="75"/>
+      <c r="C38" s="75">
         <v>20211229</v>
       </c>
-      <c r="D38" s="77"/>
+      <c r="D38" s="76"/>
     </row>
     <row r="39" customHeight="1" spans="1:4">
-      <c r="A39" s="77" t="s">
+      <c r="A39" s="76" t="s">
         <v>43</v>
       </c>
-      <c r="B39" s="76"/>
-      <c r="C39" s="76">
+      <c r="B39" s="75"/>
+      <c r="C39" s="75">
         <v>20211229</v>
       </c>
-      <c r="D39" s="77"/>
+      <c r="D39" s="76"/>
     </row>
     <row r="40" customHeight="1" spans="1:4">
-      <c r="A40" s="77" t="s">
+      <c r="A40" s="76" t="s">
         <v>44</v>
       </c>
-      <c r="B40" s="76"/>
-      <c r="C40" s="76">
+      <c r="B40" s="75"/>
+      <c r="C40" s="75">
         <v>20211230</v>
       </c>
-      <c r="D40" s="77"/>
+      <c r="D40" s="76"/>
     </row>
     <row r="41" customHeight="1" spans="1:4">
-      <c r="A41" s="77" t="s">
+      <c r="A41" s="76" t="s">
         <v>45</v>
       </c>
-      <c r="B41" s="76"/>
-      <c r="C41" s="76">
+      <c r="B41" s="75"/>
+      <c r="C41" s="75">
         <v>20220101</v>
       </c>
-      <c r="D41" s="77"/>
+      <c r="D41" s="76"/>
     </row>
     <row r="42" customHeight="1" spans="1:4">
-      <c r="A42" s="77" t="s">
+      <c r="A42" s="76" t="s">
         <v>46</v>
       </c>
-      <c r="B42" s="76"/>
-      <c r="C42" s="76">
+      <c r="B42" s="75"/>
+      <c r="C42" s="75">
         <v>20220102</v>
       </c>
-      <c r="D42" s="77"/>
+      <c r="D42" s="76"/>
     </row>
     <row r="43" customHeight="1" spans="1:4">
-      <c r="A43" s="77" t="s">
+      <c r="A43" s="76" t="s">
         <v>47</v>
       </c>
-      <c r="B43" s="76"/>
-      <c r="C43" s="76">
+      <c r="B43" s="75"/>
+      <c r="C43" s="75">
         <v>20220106</v>
       </c>
-      <c r="D43" s="77"/>
+      <c r="D43" s="76"/>
     </row>
     <row r="44" customHeight="1" spans="1:4">
-      <c r="A44" s="77" t="s">
+      <c r="A44" s="76" t="s">
         <v>48</v>
       </c>
-      <c r="B44" s="76"/>
-      <c r="C44" s="76">
+      <c r="B44" s="75"/>
+      <c r="C44" s="75">
         <v>20220108</v>
       </c>
-      <c r="D44" s="77"/>
+      <c r="D44" s="76"/>
     </row>
     <row r="45" customHeight="1" spans="1:4">
-      <c r="A45" s="77" t="s">
+      <c r="A45" s="76" t="s">
         <v>49</v>
       </c>
-      <c r="B45" s="76"/>
-      <c r="C45" s="76">
+      <c r="B45" s="75"/>
+      <c r="C45" s="75">
         <v>20220108</v>
       </c>
-      <c r="D45" s="77"/>
+      <c r="D45" s="76"/>
     </row>
     <row r="46" customHeight="1" spans="1:4">
-      <c r="A46" s="77" t="s">
+      <c r="A46" s="76" t="s">
         <v>50</v>
       </c>
-      <c r="B46" s="76"/>
-      <c r="C46" s="76">
+      <c r="B46" s="75"/>
+      <c r="C46" s="75">
         <v>20220130</v>
       </c>
-      <c r="D46" s="77"/>
+      <c r="D46" s="76"/>
     </row>
     <row r="47" customHeight="1" spans="1:4">
-      <c r="A47" s="77" t="s">
+      <c r="A47" s="76" t="s">
         <v>51</v>
       </c>
-      <c r="B47" s="76"/>
-      <c r="C47" s="76">
+      <c r="B47" s="75"/>
+      <c r="C47" s="75">
         <v>20220208</v>
       </c>
-      <c r="D47" s="77"/>
+      <c r="D47" s="76"/>
     </row>
     <row r="48" customHeight="1" spans="1:4">
-      <c r="A48" s="77" t="s">
+      <c r="A48" s="76" t="s">
         <v>52</v>
       </c>
-      <c r="B48" s="76"/>
-      <c r="C48" s="76">
+      <c r="B48" s="75"/>
+      <c r="C48" s="75">
         <v>20220210</v>
       </c>
-      <c r="D48" s="77"/>
+      <c r="D48" s="76"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
@@ -19404,28 +19448,28 @@
   </cols>
   <sheetData>
     <row r="1" ht="62" customHeight="1" spans="1:8">
-      <c r="A1" s="71" t="s">
+      <c r="A1" s="70" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="71" t="s">
+      <c r="B1" s="70" t="s">
         <v>54</v>
       </c>
-      <c r="C1" s="71" t="s">
+      <c r="C1" s="70" t="s">
         <v>55</v>
       </c>
-      <c r="D1" s="71" t="s">
+      <c r="D1" s="70" t="s">
         <v>56</v>
       </c>
-      <c r="E1" s="71" t="s">
+      <c r="E1" s="70" t="s">
         <v>57</v>
       </c>
-      <c r="F1" s="71" t="s">
+      <c r="F1" s="70" t="s">
         <v>58</v>
       </c>
-      <c r="G1" s="71" t="s">
+      <c r="G1" s="70" t="s">
         <v>59</v>
       </c>
-      <c r="H1" s="71" t="s">
+      <c r="H1" s="70" t="s">
         <v>60</v>
       </c>
     </row>
@@ -19812,10 +19856,10 @@
       <c r="D2" s="40" t="s">
         <v>139</v>
       </c>
-      <c r="E2" s="69" t="s">
+      <c r="E2" s="68" t="s">
         <v>140</v>
       </c>
-      <c r="F2" s="70"/>
+      <c r="F2" s="69"/>
     </row>
     <row r="3" ht="68" spans="1:6">
       <c r="A3" s="11"/>
@@ -19826,10 +19870,10 @@
       <c r="D3" s="40" t="s">
         <v>142</v>
       </c>
-      <c r="E3" s="69" t="s">
+      <c r="E3" s="68" t="s">
         <v>143</v>
       </c>
-      <c r="F3" s="70"/>
+      <c r="F3" s="69"/>
     </row>
     <row r="4" ht="68" spans="1:6">
       <c r="A4" s="11"/>
@@ -19840,8 +19884,8 @@
       <c r="D4" s="40" t="s">
         <v>145</v>
       </c>
-      <c r="E4" s="69"/>
-      <c r="F4" s="70"/>
+      <c r="E4" s="68"/>
+      <c r="F4" s="69"/>
     </row>
     <row r="5" ht="82" spans="1:6">
       <c r="A5" s="11"/>
@@ -19852,10 +19896,10 @@
       <c r="D5" s="52" t="s">
         <v>147</v>
       </c>
-      <c r="E5" s="69" t="s">
+      <c r="E5" s="68" t="s">
         <v>148</v>
       </c>
-      <c r="F5" s="70"/>
+      <c r="F5" s="69"/>
     </row>
     <row r="6" ht="247" spans="1:6">
       <c r="A6" s="11"/>
@@ -19866,8 +19910,8 @@
       <c r="D6" s="52" t="s">
         <v>150</v>
       </c>
-      <c r="E6" s="69"/>
-      <c r="F6" s="70"/>
+      <c r="E6" s="68"/>
+      <c r="F6" s="69"/>
     </row>
     <row r="7" ht="149" spans="1:6">
       <c r="A7" s="13"/>
@@ -19878,8 +19922,8 @@
       <c r="D7" s="52" t="s">
         <v>152</v>
       </c>
-      <c r="E7" s="69"/>
-      <c r="F7" s="70"/>
+      <c r="E7" s="68"/>
+      <c r="F7" s="69"/>
     </row>
     <row r="8" customHeight="1" spans="1:6">
       <c r="A8" s="9">
@@ -19894,8 +19938,8 @@
       <c r="D8" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="E8" s="69"/>
-      <c r="F8" s="70"/>
+      <c r="E8" s="68"/>
+      <c r="F8" s="69"/>
     </row>
     <row r="9" ht="52" customHeight="1" spans="1:6">
       <c r="A9" s="11"/>
@@ -20260,8 +20304,8 @@
   <sheetPr/>
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F6" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.5625" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -20312,7 +20356,7 @@
       <c r="G2" s="67" t="s">
         <v>215</v>
       </c>
-      <c r="H2" s="68" t="s">
+      <c r="H2" s="5" t="s">
         <v>216</v>
       </c>
     </row>
@@ -20438,7 +20482,7 @@
       <c r="G9" s="67" t="s">
         <v>237</v>
       </c>
-      <c r="H9" s="68" t="s">
+      <c r="H9" s="5" t="s">
         <v>238</v>
       </c>
     </row>
@@ -20693,13 +20737,13 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView topLeftCell="F6" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:B8"/>
+    <sheetView tabSelected="1" topLeftCell="G5" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.5625" defaultRowHeight="40" customHeight="1" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="20.5625" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
   <cols>
     <col min="1" max="1" width="20.5625" style="1" customWidth="1"/>
     <col min="2" max="2" width="35.78125" style="1" customWidth="1"/>
@@ -20798,7 +20842,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="6" s="1" customFormat="1" ht="137" customHeight="1" spans="1:7">
+    <row r="6" s="1" customFormat="1" ht="137" customHeight="1" spans="1:8">
       <c r="A6" s="9">
         <v>4.2</v>
       </c>
@@ -20818,6 +20862,7 @@
       <c r="G6" s="40" t="s">
         <v>283</v>
       </c>
+      <c r="H6"/>
     </row>
     <row r="7" s="1" customFormat="1" ht="66" customHeight="1" spans="1:7">
       <c r="A7" s="11"/>
@@ -21082,7 +21127,8 @@
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
-  <legacyDrawing r:id="rId2"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Mon Apr  4 14:48:20 CST 2022
</commit_message>
<xml_diff>
--- a/笔记/CBAP/知识点.xlsx
+++ b/笔记/CBAP/知识点.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="13180" activeTab="6"/>
+    <workbookView windowWidth="28800" windowHeight="13180"/>
   </bookViews>
   <sheets>
     <sheet name="核查单" sheetId="12" r:id="rId1"/>
@@ -11771,10 +11771,10 @@
   <sheetPr/>
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D33" sqref="D33"/>
+      <selection pane="bottomLeft" activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.703125" defaultRowHeight="40" customHeight="1" outlineLevelCol="3"/>
@@ -12111,9 +12111,11 @@
       <c r="A34" s="77" t="s">
         <v>38</v>
       </c>
-      <c r="B34" s="77"/>
-      <c r="C34" s="77"/>
-      <c r="D34" s="77"/>
+      <c r="B34" s="76"/>
+      <c r="C34" s="76">
+        <v>20220402</v>
+      </c>
+      <c r="D34" s="76"/>
     </row>
     <row r="35" customHeight="1" spans="1:4">
       <c r="A35" s="77" t="s">
@@ -12268,7 +12270,7 @@
   <sheetPr/>
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView topLeftCell="F13" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
@@ -20347,7 +20349,7 @@
   <sheetPr/>
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="B5" sqref="B5:B8"/>
     </sheetView>
   </sheetViews>
@@ -21183,8 +21185,8 @@
   <sheetPr/>
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G15" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView topLeftCell="B18" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.5625" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -21692,7 +21694,7 @@
   <sheetPr/>
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A20" workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
@@ -22188,7 +22190,7 @@
   <sheetPr/>
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView topLeftCell="F17" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>

</xml_diff>